<commit_message>
loading actions_list which replaces own/mob actx
</commit_message>
<xml_diff>
--- a/level_actions.xlsx
+++ b/level_actions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madma\Documents\pyGurly\pyGurly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4918E476-2191-420E-8BA0-612E37AAA892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AD57C8-4C17-4153-8E50-0644CEE86EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="level_actions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>Punch</t>
   </si>
@@ -167,12 +180,39 @@
   </si>
   <si>
     <t>ABVavg hit calc</t>
+  </si>
+  <si>
+    <t>Gaseous Punishment</t>
+  </si>
+  <si>
+    <t>Copper Sword</t>
+  </si>
+  <si>
+    <t>Nunchucks</t>
+  </si>
+  <si>
+    <t>Copper Axe</t>
+  </si>
+  <si>
+    <t>Simple Hammer</t>
+  </si>
+  <si>
+    <t>Monster1</t>
+  </si>
+  <si>
+    <t>Monster2</t>
+  </si>
+  <si>
+    <t>Monster3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -650,8 +690,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1006,20 +1047,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1064,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1124,7 +1166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -1164,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1184,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1204,7 +1246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -1224,7 +1266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -1244,7 +1286,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>29</v>
       </c>
@@ -1252,7 +1294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -1314,7 +1356,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1327,10 +1369,10 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
       <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
         <v>1</v>
       </c>
       <c r="R16">
@@ -1352,8 +1394,12 @@
         <f>C16</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z16" s="1">
+        <f>AVERAGE(V16:X16)/Y16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1397,8 +1443,12 @@
         <f t="shared" ref="Y17:Y26" si="3">C17</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17" s="1">
+        <f t="shared" ref="Z17:Z28" si="4">AVERAGE(V17:X17)/Y17</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1439,8 +1489,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1459,7 +1513,7 @@
       <c r="M19">
         <v>1</v>
       </c>
-      <c r="P19">
+      <c r="O19">
         <v>1</v>
       </c>
       <c r="R19">
@@ -1481,8 +1535,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19" s="1"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1490,7 +1545,7 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1521,10 +1576,14 @@
       </c>
       <c r="Y20">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1565,8 +1624,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21" s="1"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1607,8 +1667,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22" s="1"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1624,30 +1685,37 @@
       <c r="I23">
         <v>1</v>
       </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
       <c r="P23">
         <v>1</v>
       </c>
       <c r="R23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="V23">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W23">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X23">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y23">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1682,8 +1750,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z24" s="1"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -1718,8 +1787,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -1735,24 +1805,37 @@
       <c r="J26" t="s">
         <v>37</v>
       </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>6</v>
+      </c>
       <c r="V26">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="X26">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Y26">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26" s="1">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
@@ -1781,84 +1864,410 @@
         <v>6</v>
       </c>
       <c r="V27">
-        <f t="shared" ref="V27" si="4">(5*SUM(D27:I27))-(5*SUM(L27:Q27))+R27</f>
+        <f t="shared" ref="V27" si="5">(5*SUM(D27:I27))-(5*SUM(L27:Q27))+R27</f>
         <v>6</v>
       </c>
       <c r="W27">
-        <f t="shared" ref="W27" si="5">(3*SUM(D27:I27))-(5*SUM(L27:Q27))+R27</f>
+        <f t="shared" ref="W27" si="6">(3*SUM(D27:I27))-(5*SUM(L27:Q27))+R27</f>
         <v>0</v>
       </c>
       <c r="X27">
-        <f t="shared" ref="X27" si="6">(7*SUM(D27:I27))-(5*SUM(L27:Q27))+R27</f>
+        <f t="shared" ref="X27" si="7">(7*SUM(D27:I27))-(5*SUM(L27:Q27))+R27</f>
         <v>12</v>
       </c>
       <c r="Y27">
-        <f t="shared" ref="Y27" si="7">C27</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Y27" si="8">C27</f>
+        <v>2</v>
+      </c>
+      <c r="Z27" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>6</v>
+      </c>
+      <c r="V28">
+        <f t="shared" ref="V28" si="9">(5*SUM(D28:I28))-(5*SUM(L28:Q28))+R28</f>
+        <v>6</v>
+      </c>
+      <c r="W28">
+        <f t="shared" ref="W28" si="10">(3*SUM(D28:I28))-(5*SUM(L28:Q28))+R28</f>
+        <v>2</v>
+      </c>
+      <c r="X28">
+        <f t="shared" ref="X28" si="11">(7*SUM(D28:I28))-(5*SUM(L28:Q28))+R28</f>
+        <v>10</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" ref="Y28" si="12">C28</f>
+        <v>2</v>
+      </c>
+      <c r="Z28" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>10</v>
+      </c>
+      <c r="V29">
+        <f t="shared" ref="V29:V35" si="13">(5*SUM(D29:I29))-(5*SUM(L29:Q29))+R29</f>
+        <v>5</v>
+      </c>
+      <c r="W29">
+        <f t="shared" ref="W29:W35" si="14">(3*SUM(D29:I29))-(5*SUM(L29:Q29))+R29</f>
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <f t="shared" ref="X29:X35" si="15">(7*SUM(D29:I29))-(5*SUM(L29:Q29))+R29</f>
+        <v>7</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Y35" si="16">C29</f>
+        <v>2</v>
+      </c>
+      <c r="Z29" s="1">
+        <f t="shared" ref="Z29:Z35" si="17">AVERAGE(V29:X29)/Y29</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>10</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Z30" s="1">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>6</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="14"/>
+        <v>-1</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Z31" s="1">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="R32">
+        <v>10</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="14"/>
+        <v>-1</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="Z32" s="1">
+        <f t="shared" si="17"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>6</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Z33" s="1">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <v>10</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Z34" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="R35">
+        <v>6</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="Z35" s="1">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Y16:Y27">
+  <conditionalFormatting sqref="Y16:Y35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>